<commit_message>
update README and delete excel data
</commit_message>
<xml_diff>
--- a/Marklist.xlsx
+++ b/Marklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/megha.jayakumar/Desktop/Python Projects/Student grades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED66343-55A8-D04D-B97B-032831B0DBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CB7971-F8AA-FD44-8DE1-B06BD973BDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12 a" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Student ID</t>
   </si>
@@ -42,18 +42,6 @@
   </si>
   <si>
     <t>Percentage</t>
-  </si>
-  <si>
-    <t>Abhiram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gouri </t>
-  </si>
-  <si>
-    <t>Megha</t>
-  </si>
-  <si>
-    <t>Sanika</t>
   </si>
 </sst>
 </file>
@@ -393,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="168" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -424,52 +412,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>204</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2">
-        <v>99</v>
-      </c>
-      <c r="E2">
-        <v>96</v>
-      </c>
-      <c r="F2">
-        <v>92</v>
-      </c>
-      <c r="G2">
-        <v>96.75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>205</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>97</v>
-      </c>
-      <c r="D3">
-        <v>96</v>
-      </c>
-      <c r="E3">
-        <v>93</v>
-      </c>
-      <c r="F3">
-        <v>94</v>
-      </c>
-      <c r="G3">
-        <v>95</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -477,10 +419,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView zoomScale="161" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
+      <selection activeCell="G5" sqref="A2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -508,52 +450,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>287</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>99</v>
-      </c>
-      <c r="D2">
-        <v>98</v>
-      </c>
-      <c r="E2">
-        <v>95</v>
-      </c>
-      <c r="F2">
-        <v>92</v>
-      </c>
-      <c r="G2">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>210</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>99</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3">
-        <v>95</v>
-      </c>
-      <c r="F3">
-        <v>93</v>
-      </c>
-      <c r="G3">
-        <v>96.75</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>